<commit_message>
Verificar el login y el buscar
</commit_message>
<xml_diff>
--- a/RetoDatos.xlsx
+++ b/RetoDatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpala\IdeaProjects\RetoSemilleroSqa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3E58D6-AA8A-4B7C-83C6-42298FACFC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0B092-247F-42CC-A721-3EE82EBA5D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{EB043CE5-115F-4DE3-A4AE-AA0462BA3004}"/>
+    <workbookView xWindow="4035" yWindow="1380" windowWidth="15375" windowHeight="7875" xr2:uid="{EB043CE5-115F-4DE3-A4AE-AA0462BA3004}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosLogueo" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,9 +40,6 @@
     <t>hpalaciom.1997@gmail.com</t>
   </si>
   <si>
-    <t>Hpalacio1997</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
@@ -54,6 +50,9 @@
   </si>
   <si>
     <t>Balones</t>
+  </si>
+  <si>
+    <t>Hpalacio1997</t>
   </si>
 </sst>
 </file>
@@ -112,13 +111,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -436,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4220FC72-2643-4656-BC0E-6B5800E235F5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,10 +450,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -479,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DB0FB5-FD09-4592-A10F-1C87D8C8205D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -490,12 +488,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>